<commit_message>
bom fixed(510k resistor-> 510 resistor)
</commit_message>
<xml_diff>
--- a/bom.xlsx
+++ b/bom.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="24960" windowHeight="15000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="100">
   <si>
     <t>TOGGLE SWITCH</t>
   </si>
@@ -162,9 +162,6 @@
     <t>Standard resistor, various versions</t>
   </si>
   <si>
-    <t>R9, R10, R37</t>
-  </si>
-  <si>
     <t>10MM_RESISTOR</t>
   </si>
   <si>
@@ -180,12 +177,6 @@
     <t>470k</t>
   </si>
   <si>
-    <t>R49</t>
-  </si>
-  <si>
-    <t>510k</t>
-  </si>
-  <si>
     <t>R40</t>
   </si>
   <si>
@@ -325,6 +316,9 @@
   </si>
   <si>
     <t>SSM2164P(Coolaudio's v2164d would be another choice)</t>
+  </si>
+  <si>
+    <t>R9, R10, R37, R49</t>
   </si>
 </sst>
 </file>
@@ -705,10 +699,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F37"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -722,27 +716,27 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -755,19 +749,19 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -775,19 +769,19 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -795,19 +789,19 @@
         <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>87</v>
-      </c>
       <c r="F5" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -815,24 +809,24 @@
         <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -845,24 +839,24 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -875,24 +869,24 @@
         <v>6</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -905,16 +899,16 @@
         <v>9</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>46</v>
@@ -925,16 +919,16 @@
         <v>6</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>46</v>
@@ -945,16 +939,16 @@
         <v>1</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>46</v>
@@ -965,16 +959,16 @@
         <v>1</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>46</v>
@@ -985,16 +979,16 @@
         <v>6</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>46</v>
@@ -1005,16 +999,16 @@
         <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>46</v>
@@ -1025,16 +1019,16 @@
         <v>1</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>46</v>
@@ -1045,16 +1039,16 @@
         <v>1</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>46</v>
@@ -1065,16 +1059,16 @@
         <v>1</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>46</v>
@@ -1082,19 +1076,19 @@
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>52</v>
+        <v>17</v>
       </c>
       <c r="C21" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>46</v>
@@ -1102,72 +1096,72 @@
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="1">
-        <v>5</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>17</v>
+        <v>4</v>
+      </c>
+      <c r="B22" s="1">
+        <v>510</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>50</v>
+        <v>99</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="1">
-        <v>3</v>
-      </c>
-      <c r="B23" s="1">
-        <v>510</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>46</v>
-      </c>
+      <c r="A23" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
     </row>
     <row r="24" spans="1:6">
-      <c r="A24" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
+      <c r="A24" s="1">
+        <v>1</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="1">
         <v>1</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>37</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -1175,69 +1169,69 @@
         <v>1</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>37</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="27" spans="1:6">
-      <c r="A27" s="1">
-        <v>1</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>35</v>
-      </c>
+      <c r="A27" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
     </row>
     <row r="28" spans="1:6">
-      <c r="A28" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
+      <c r="A28" s="1">
+        <v>3</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -1245,19 +1239,19 @@
         <v>1</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>98</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -1265,87 +1259,87 @@
         <v>1</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>101</v>
+        <v>22</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>21</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="32" spans="1:6">
-      <c r="A32" s="1">
-        <v>1</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>19</v>
-      </c>
+      <c r="A32" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
     </row>
     <row r="33" spans="1:6">
-      <c r="A33" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
+      <c r="A33" s="1">
+        <v>11</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" s="1">
+        <v>12</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D34" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B34" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="E34" s="1"/>
       <c r="F34" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" s="1">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E35" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="F35" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -1353,38 +1347,18 @@
         <v>1</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6">
-      <c r="A37" s="1">
-        <v>1</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F37" s="1" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Revert "bom fixed(510k resistor-> 510 resistor)"
This reverts commit df4ec627675dfb7104e617b637165430886ac1f1.
</commit_message>
<xml_diff>
--- a/bom.xlsx
+++ b/bom.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15560" tabRatio="500"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="24960" windowHeight="15000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="102">
   <si>
     <t>TOGGLE SWITCH</t>
   </si>
@@ -162,6 +162,9 @@
     <t>Standard resistor, various versions</t>
   </si>
   <si>
+    <t>R9, R10, R37</t>
+  </si>
+  <si>
     <t>10MM_RESISTOR</t>
   </si>
   <si>
@@ -177,6 +180,12 @@
     <t>470k</t>
   </si>
   <si>
+    <t>R49</t>
+  </si>
+  <si>
+    <t>510k</t>
+  </si>
+  <si>
     <t>R40</t>
   </si>
   <si>
@@ -316,9 +325,6 @@
   </si>
   <si>
     <t>SSM2164P(Coolaudio's v2164d would be another choice)</t>
-  </si>
-  <si>
-    <t>R9, R10, R37, R49</t>
   </si>
 </sst>
 </file>
@@ -699,10 +705,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F36"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -716,27 +722,27 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -749,19 +755,19 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -769,19 +775,19 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -789,19 +795,19 @@
         <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -809,24 +815,24 @@
         <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="2" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -839,24 +845,24 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -869,24 +875,24 @@
         <v>6</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="2" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -899,16 +905,16 @@
         <v>9</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>47</v>
-      </c>
       <c r="E12" s="1" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>46</v>
@@ -919,16 +925,16 @@
         <v>6</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>47</v>
-      </c>
       <c r="E13" s="1" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>46</v>
@@ -939,16 +945,16 @@
         <v>1</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>47</v>
-      </c>
       <c r="E14" s="1" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>46</v>
@@ -959,16 +965,16 @@
         <v>1</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C15" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>47</v>
-      </c>
       <c r="E15" s="1" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>46</v>
@@ -979,16 +985,16 @@
         <v>6</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>47</v>
-      </c>
       <c r="E16" s="1" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>46</v>
@@ -999,16 +1005,16 @@
         <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C17" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>47</v>
-      </c>
       <c r="E17" s="1" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>46</v>
@@ -1019,16 +1025,16 @@
         <v>1</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C18" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>47</v>
-      </c>
       <c r="E18" s="1" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>46</v>
@@ -1039,16 +1045,16 @@
         <v>1</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="C19" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D19" s="1" t="s">
-        <v>47</v>
-      </c>
       <c r="E19" s="1" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>46</v>
@@ -1059,16 +1065,16 @@
         <v>1</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C20" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>47</v>
-      </c>
       <c r="E20" s="1" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>46</v>
@@ -1076,19 +1082,19 @@
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>17</v>
+        <v>52</v>
       </c>
       <c r="C21" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>47</v>
-      </c>
       <c r="E21" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>46</v>
@@ -1096,72 +1102,72 @@
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="1">
-        <v>4</v>
-      </c>
-      <c r="B22" s="1">
-        <v>510</v>
+        <v>5</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="C22" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D22" s="1" t="s">
-        <v>47</v>
-      </c>
       <c r="E22" s="1" t="s">
-        <v>99</v>
+        <v>50</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="1">
+        <v>3</v>
+      </c>
+      <c r="B23" s="1">
+        <v>510</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" s="1">
-        <v>1</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>42</v>
-      </c>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="1">
         <v>1</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>37</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -1169,69 +1175,69 @@
         <v>1</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>37</v>
       </c>
       <c r="E26" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="1">
+        <v>1</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E27" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F26" s="1" t="s">
+      <c r="F27" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
-      <c r="A27" s="2" t="s">
+    <row r="28" spans="1:6">
+      <c r="A28" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-    </row>
-    <row r="28" spans="1:6">
-      <c r="A28" s="1">
-        <v>3</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -1239,19 +1245,19 @@
         <v>1</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>98</v>
+        <v>29</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -1259,87 +1265,87 @@
         <v>1</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>101</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>21</v>
       </c>
       <c r="E31" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" s="1">
+        <v>1</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E32" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F31" s="1" t="s">
+      <c r="F32" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
-      <c r="A32" s="2" t="s">
+    <row r="33" spans="1:6">
+      <c r="A33" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-    </row>
-    <row r="33" spans="1:6">
-      <c r="A33" s="1">
-        <v>11</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>13</v>
-      </c>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" s="1">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E34" s="1"/>
+        <v>15</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="F34" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" s="1">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>6</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="E35" s="1"/>
       <c r="F35" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -1347,18 +1353,38 @@
         <v>1</v>
       </c>
       <c r="B36" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" s="1">
+        <v>1</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C37" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="D37" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E36" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F36" s="1" t="s">
+      <c r="E37" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F37" s="1" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed R49 from 510k into 510
</commit_message>
<xml_diff>
--- a/bom.xlsx
+++ b/bom.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="24960" windowHeight="15000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="100">
   <si>
     <t>TOGGLE SWITCH</t>
   </si>
@@ -162,9 +162,6 @@
     <t>Standard resistor, various versions</t>
   </si>
   <si>
-    <t>R9, R10, R37</t>
-  </si>
-  <si>
     <t>10MM_RESISTOR</t>
   </si>
   <si>
@@ -180,12 +177,6 @@
     <t>470k</t>
   </si>
   <si>
-    <t>R49</t>
-  </si>
-  <si>
-    <t>510k</t>
-  </si>
-  <si>
     <t>R40</t>
   </si>
   <si>
@@ -325,6 +316,9 @@
   </si>
   <si>
     <t>SSM2164P(Coolaudio's v2164d would be another choice)</t>
+  </si>
+  <si>
+    <t>R9, R10, R37, R49</t>
   </si>
 </sst>
 </file>
@@ -705,10 +699,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F37"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -722,27 +716,27 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -755,19 +749,19 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -775,19 +769,19 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -795,19 +789,19 @@
         <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>87</v>
-      </c>
       <c r="F5" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -815,24 +809,24 @@
         <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -845,24 +839,24 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -875,24 +869,24 @@
         <v>6</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -905,16 +899,16 @@
         <v>9</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>46</v>
@@ -925,16 +919,16 @@
         <v>6</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>46</v>
@@ -945,16 +939,16 @@
         <v>1</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>46</v>
@@ -965,16 +959,16 @@
         <v>1</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>46</v>
@@ -985,16 +979,16 @@
         <v>6</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>46</v>
@@ -1005,16 +999,16 @@
         <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>46</v>
@@ -1025,16 +1019,16 @@
         <v>1</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>46</v>
@@ -1045,16 +1039,16 @@
         <v>1</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>46</v>
@@ -1065,16 +1059,16 @@
         <v>1</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>46</v>
@@ -1082,19 +1076,19 @@
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>52</v>
+        <v>17</v>
       </c>
       <c r="C21" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>46</v>
@@ -1102,72 +1096,72 @@
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="1">
-        <v>5</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>17</v>
+        <v>4</v>
+      </c>
+      <c r="B22" s="1">
+        <v>510</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>50</v>
+        <v>99</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="1">
-        <v>3</v>
-      </c>
-      <c r="B23" s="1">
-        <v>510</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>46</v>
-      </c>
+      <c r="A23" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
     </row>
     <row r="24" spans="1:6">
-      <c r="A24" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
+      <c r="A24" s="1">
+        <v>1</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="1">
         <v>1</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>37</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -1175,69 +1169,69 @@
         <v>1</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>37</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="27" spans="1:6">
-      <c r="A27" s="1">
-        <v>1</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>35</v>
-      </c>
+      <c r="A27" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
     </row>
     <row r="28" spans="1:6">
-      <c r="A28" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
+      <c r="A28" s="1">
+        <v>3</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -1245,19 +1239,19 @@
         <v>1</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>98</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -1265,87 +1259,87 @@
         <v>1</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>101</v>
+        <v>22</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>21</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="32" spans="1:6">
-      <c r="A32" s="1">
-        <v>1</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>19</v>
-      </c>
+      <c r="A32" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
     </row>
     <row r="33" spans="1:6">
-      <c r="A33" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
+      <c r="A33" s="1">
+        <v>11</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" s="1">
+        <v>12</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D34" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B34" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="E34" s="1"/>
       <c r="F34" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" s="1">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E35" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="F35" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -1353,38 +1347,18 @@
         <v>1</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6">
-      <c r="A37" s="1">
-        <v>1</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F37" s="1" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
BOM details updated & recommendation
</commit_message>
<xml_diff>
--- a/bom.xlsx
+++ b/bom.xlsx
@@ -11,9 +11,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="98">
-  <si>
-    <t>DIY Eurorack Benjolin by Kweiwen BOM</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="99">
+  <si>
+    <t>DIY Eurorack Benjolin BOM by Kweiwen</t>
   </si>
   <si>
     <t>Qty</t>
@@ -305,6 +305,87 @@
   </si>
   <si>
     <t>8-bit Static SHIFT REGISTER</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>Frequently Asked Quesiotns: + +</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>Q: Where can i get quad vca?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">A: V2164 at Thonk, Electric Druid; SSM2164 at Synthcube + +Q: Where can i get 9mm potentiometers?
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">A: Thonk, Mouser, Small Bear, Modular Addict… + +Q: Where can i get pj301m-12?
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">A: Thonk, Modular Addict, Synthrotek… + +Q: Rest parts?
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>A: Your local electric store + +</t>
+    </r>
+    <r>
+      <rPr>
+        <i val="1"/>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>*recommend R18 with 62k instead of 47k, which would have a better result*</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -314,7 +395,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -335,6 +416,12 @@
       <color indexed="8"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <i val="1"/>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -351,18 +438,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="12"/>
+        <fgColor indexed="11"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="14"/>
+        <fgColor indexed="12"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -379,7 +466,7 @@
         <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="11"/>
+        <color indexed="8"/>
       </bottom>
       <diagonal/>
     </border>
@@ -390,7 +477,7 @@
         <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="11"/>
+        <color indexed="8"/>
       </bottom>
       <diagonal/>
     </border>
@@ -403,19 +490,108 @@
         <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="11"/>
+        <color indexed="8"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="11"/>
+        <color indexed="8"/>
       </left>
       <right style="thin">
-        <color indexed="11"/>
+        <color indexed="8"/>
       </right>
       <top style="thin">
-        <color indexed="11"/>
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="13"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="13"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
         <color indexed="13"/>
@@ -424,91 +600,91 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="11"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="13"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
         <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="11"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="13"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="11"/>
+        <color indexed="9"/>
       </right>
       <top style="thin">
         <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="11"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="11"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="11"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="13"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="11"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="11"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="13"/>
+        <color indexed="9"/>
       </right>
       <top style="thin">
-        <color indexed="11"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="11"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="13"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="11"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="11"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="11"/>
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="11"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="11"/>
+        <color indexed="9"/>
       </right>
       <top style="thin">
-        <color indexed="11"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="11"/>
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
@@ -518,7 +694,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -537,26 +713,62 @@
     <xf numFmtId="49" fontId="3" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -577,10 +789,9 @@
       <rgbColor rgb="ff000000"/>
       <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="ffbdc0bf"/>
+      <rgbColor rgb="ffdbdbdb"/>
       <rgbColor rgb="ffa5a5a5"/>
-      <rgbColor rgb="ffbdc0bf"/>
-      <rgbColor rgb="ff3f3f3f"/>
-      <rgbColor rgb="ffdbdbdb"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -1645,18 +1856,18 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.33333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.33333" defaultRowHeight="13.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="4.35156" style="1" customWidth="1"/>
     <col min="2" max="2" width="13.1719" style="1" customWidth="1"/>
     <col min="3" max="3" width="18.6719" style="1" customWidth="1"/>
     <col min="4" max="4" width="25.3516" style="1" customWidth="1"/>
     <col min="5" max="5" width="69.5" style="1" customWidth="1"/>
-    <col min="6" max="6" width="44.4688" style="1" customWidth="1"/>
+    <col min="6" max="6" width="44.5" style="1" customWidth="1"/>
     <col min="7" max="256" width="8.35156" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1697,516 +1908,516 @@
       <c r="B3" t="s" s="7">
         <v>7</v>
       </c>
-      <c r="C3" t="s" s="8">
+      <c r="C3" t="s" s="7">
         <v>8</v>
       </c>
-      <c r="D3" t="s" s="8">
+      <c r="D3" t="s" s="7">
         <v>9</v>
       </c>
-      <c r="E3" t="s" s="8">
+      <c r="E3" t="s" s="7">
         <v>10</v>
       </c>
-      <c r="F3" t="s" s="8">
+      <c r="F3" t="s" s="7">
         <v>11</v>
       </c>
     </row>
     <row r="4" ht="20.05" customHeight="1">
-      <c r="A4" s="9">
+      <c r="A4" s="6">
         <v>5</v>
       </c>
-      <c r="B4" t="s" s="10">
+      <c r="B4" t="s" s="7">
         <v>12</v>
       </c>
-      <c r="C4" t="s" s="11">
+      <c r="C4" t="s" s="7">
         <v>13</v>
       </c>
-      <c r="D4" t="s" s="11">
+      <c r="D4" t="s" s="7">
         <v>14</v>
       </c>
-      <c r="E4" t="s" s="11">
+      <c r="E4" t="s" s="7">
         <v>15</v>
       </c>
-      <c r="F4" t="s" s="11">
+      <c r="F4" t="s" s="7">
         <v>16</v>
       </c>
     </row>
     <row r="5" ht="20.05" customHeight="1">
-      <c r="A5" s="9">
+      <c r="A5" s="6">
         <v>2</v>
       </c>
-      <c r="B5" t="s" s="10">
+      <c r="B5" t="s" s="7">
         <v>17</v>
       </c>
-      <c r="C5" t="s" s="11">
+      <c r="C5" t="s" s="7">
         <v>13</v>
       </c>
-      <c r="D5" t="s" s="11">
+      <c r="D5" t="s" s="7">
         <v>14</v>
       </c>
-      <c r="E5" t="s" s="11">
+      <c r="E5" t="s" s="7">
         <v>18</v>
       </c>
-      <c r="F5" t="s" s="11">
+      <c r="F5" t="s" s="7">
         <v>19</v>
       </c>
     </row>
     <row r="6" ht="20.05" customHeight="1">
-      <c r="A6" s="9">
+      <c r="A6" s="6">
         <v>3</v>
       </c>
-      <c r="B6" t="s" s="10">
+      <c r="B6" t="s" s="7">
         <v>20</v>
       </c>
-      <c r="C6" t="s" s="11">
+      <c r="C6" t="s" s="7">
         <v>13</v>
       </c>
-      <c r="D6" t="s" s="11">
+      <c r="D6" t="s" s="7">
         <v>14</v>
       </c>
-      <c r="E6" t="s" s="11">
+      <c r="E6" t="s" s="7">
         <v>21</v>
       </c>
-      <c r="F6" t="s" s="11">
+      <c r="F6" t="s" s="7">
         <v>16</v>
       </c>
     </row>
     <row r="7" ht="20.05" customHeight="1">
-      <c r="A7" s="9">
+      <c r="A7" s="6">
         <v>4</v>
       </c>
-      <c r="B7" t="s" s="10">
+      <c r="B7" t="s" s="7">
         <v>22</v>
       </c>
-      <c r="C7" t="s" s="11">
+      <c r="C7" t="s" s="7">
         <v>13</v>
       </c>
-      <c r="D7" t="s" s="11">
+      <c r="D7" t="s" s="7">
         <v>14</v>
       </c>
-      <c r="E7" t="s" s="11">
+      <c r="E7" t="s" s="7">
         <v>23</v>
       </c>
-      <c r="F7" t="s" s="11">
+      <c r="F7" t="s" s="7">
         <v>16</v>
       </c>
     </row>
     <row r="8" ht="20.05" customHeight="1">
-      <c r="A8" s="9">
+      <c r="A8" s="6">
         <v>4</v>
       </c>
-      <c r="B8" t="s" s="10">
+      <c r="B8" t="s" s="7">
         <v>24</v>
       </c>
-      <c r="C8" t="s" s="11">
+      <c r="C8" t="s" s="7">
         <v>25</v>
       </c>
-      <c r="D8" t="s" s="11">
+      <c r="D8" t="s" s="7">
         <v>26</v>
       </c>
-      <c r="E8" t="s" s="11">
+      <c r="E8" t="s" s="7">
         <v>27</v>
       </c>
-      <c r="F8" t="s" s="11">
+      <c r="F8" t="s" s="7">
         <v>28</v>
       </c>
     </row>
     <row r="9" ht="20.05" customHeight="1">
-      <c r="A9" s="9">
+      <c r="A9" s="6">
         <v>1</v>
       </c>
-      <c r="B9" t="s" s="10">
+      <c r="B9" t="s" s="7">
         <v>29</v>
       </c>
-      <c r="C9" t="s" s="11">
+      <c r="C9" t="s" s="7">
         <v>30</v>
       </c>
-      <c r="D9" t="s" s="11">
+      <c r="D9" t="s" s="7">
         <v>31</v>
       </c>
-      <c r="E9" t="s" s="11">
+      <c r="E9" t="s" s="7">
         <v>32</v>
       </c>
-      <c r="F9" t="s" s="11">
+      <c r="F9" t="s" s="7">
         <v>33</v>
       </c>
     </row>
     <row r="10" ht="20.05" customHeight="1">
-      <c r="A10" s="9">
+      <c r="A10" s="6">
         <v>6</v>
       </c>
-      <c r="B10" t="s" s="10">
+      <c r="B10" t="s" s="7">
         <v>34</v>
       </c>
-      <c r="C10" t="s" s="11">
+      <c r="C10" t="s" s="7">
         <v>30</v>
       </c>
-      <c r="D10" t="s" s="11">
+      <c r="D10" t="s" s="7">
         <v>31</v>
       </c>
-      <c r="E10" t="s" s="11">
+      <c r="E10" t="s" s="7">
         <v>35</v>
       </c>
-      <c r="F10" t="s" s="11">
+      <c r="F10" t="s" s="7">
         <v>33</v>
       </c>
     </row>
     <row r="11" ht="20.05" customHeight="1">
-      <c r="A11" s="9">
+      <c r="A11" s="6">
         <v>5</v>
       </c>
-      <c r="B11" t="s" s="10">
+      <c r="B11" t="s" s="7">
         <v>36</v>
       </c>
-      <c r="C11" t="s" s="11">
+      <c r="C11" t="s" s="7">
         <v>30</v>
       </c>
-      <c r="D11" t="s" s="11">
+      <c r="D11" t="s" s="7">
         <v>31</v>
       </c>
-      <c r="E11" t="s" s="11">
+      <c r="E11" t="s" s="7">
         <v>37</v>
       </c>
-      <c r="F11" t="s" s="11">
+      <c r="F11" t="s" s="7">
         <v>33</v>
       </c>
     </row>
     <row r="12" ht="20.05" customHeight="1">
-      <c r="A12" s="9">
+      <c r="A12" s="6">
         <v>1</v>
       </c>
-      <c r="B12" t="s" s="10">
+      <c r="B12" t="s" s="7">
         <v>38</v>
       </c>
-      <c r="C12" t="s" s="11">
+      <c r="C12" t="s" s="7">
         <v>30</v>
       </c>
-      <c r="D12" t="s" s="11">
+      <c r="D12" t="s" s="7">
         <v>31</v>
       </c>
-      <c r="E12" t="s" s="11">
+      <c r="E12" t="s" s="7">
         <v>39</v>
       </c>
-      <c r="F12" t="s" s="11">
+      <c r="F12" t="s" s="7">
         <v>33</v>
       </c>
     </row>
     <row r="13" ht="20.05" customHeight="1">
-      <c r="A13" s="9">
+      <c r="A13" s="6">
         <v>6</v>
       </c>
-      <c r="B13" t="s" s="10">
+      <c r="B13" t="s" s="7">
         <v>40</v>
       </c>
-      <c r="C13" t="s" s="11">
+      <c r="C13" t="s" s="7">
         <v>30</v>
       </c>
-      <c r="D13" t="s" s="11">
+      <c r="D13" t="s" s="7">
         <v>31</v>
       </c>
-      <c r="E13" t="s" s="11">
+      <c r="E13" t="s" s="7">
         <v>41</v>
       </c>
-      <c r="F13" t="s" s="11">
+      <c r="F13" t="s" s="7">
         <v>33</v>
       </c>
     </row>
     <row r="14" ht="20.05" customHeight="1">
-      <c r="A14" s="9">
+      <c r="A14" s="6">
         <v>15</v>
       </c>
-      <c r="B14" t="s" s="10">
+      <c r="B14" t="s" s="7">
         <v>42</v>
       </c>
-      <c r="C14" t="s" s="11">
+      <c r="C14" t="s" s="7">
         <v>30</v>
       </c>
-      <c r="D14" t="s" s="11">
+      <c r="D14" t="s" s="7">
         <v>31</v>
       </c>
-      <c r="E14" t="s" s="11">
+      <c r="E14" t="s" s="7">
         <v>43</v>
       </c>
-      <c r="F14" t="s" s="11">
+      <c r="F14" t="s" s="7">
         <v>33</v>
       </c>
     </row>
     <row r="15" ht="20.05" customHeight="1">
-      <c r="A15" s="9">
+      <c r="A15" s="6">
         <v>1</v>
       </c>
-      <c r="B15" t="s" s="10">
+      <c r="B15" t="s" s="7">
         <v>44</v>
       </c>
-      <c r="C15" t="s" s="11">
+      <c r="C15" t="s" s="7">
         <v>30</v>
       </c>
-      <c r="D15" t="s" s="11">
+      <c r="D15" t="s" s="7">
         <v>31</v>
       </c>
-      <c r="E15" t="s" s="11">
+      <c r="E15" t="s" s="7">
         <v>45</v>
       </c>
-      <c r="F15" t="s" s="11">
+      <c r="F15" t="s" s="7">
         <v>33</v>
       </c>
     </row>
     <row r="16" ht="20.05" customHeight="1">
-      <c r="A16" s="9">
+      <c r="A16" s="6">
         <v>4</v>
       </c>
-      <c r="B16" s="12">
+      <c r="B16" s="8">
         <v>510</v>
       </c>
-      <c r="C16" t="s" s="11">
+      <c r="C16" t="s" s="7">
         <v>30</v>
       </c>
-      <c r="D16" t="s" s="11">
+      <c r="D16" t="s" s="7">
         <v>31</v>
       </c>
-      <c r="E16" t="s" s="11">
+      <c r="E16" t="s" s="7">
         <v>46</v>
       </c>
-      <c r="F16" t="s" s="11">
+      <c r="F16" t="s" s="7">
         <v>33</v>
       </c>
     </row>
     <row r="17" ht="20.05" customHeight="1">
-      <c r="A17" s="9">
+      <c r="A17" s="6">
         <v>9</v>
       </c>
-      <c r="B17" t="s" s="10">
+      <c r="B17" t="s" s="7">
         <v>47</v>
       </c>
-      <c r="C17" t="s" s="11">
+      <c r="C17" t="s" s="7">
         <v>30</v>
       </c>
-      <c r="D17" t="s" s="11">
+      <c r="D17" t="s" s="7">
         <v>31</v>
       </c>
-      <c r="E17" t="s" s="11">
+      <c r="E17" t="s" s="7">
         <v>48</v>
       </c>
-      <c r="F17" t="s" s="11">
+      <c r="F17" t="s" s="7">
         <v>33</v>
       </c>
     </row>
     <row r="18" ht="20.05" customHeight="1">
-      <c r="A18" s="9">
+      <c r="A18" s="6">
         <v>2</v>
       </c>
-      <c r="B18" t="s" s="10">
+      <c r="B18" t="s" s="7">
         <v>49</v>
       </c>
-      <c r="C18" t="s" s="11">
+      <c r="C18" t="s" s="7">
         <v>30</v>
       </c>
-      <c r="D18" t="s" s="11">
+      <c r="D18" t="s" s="7">
         <v>31</v>
       </c>
-      <c r="E18" t="s" s="11">
+      <c r="E18" t="s" s="7">
         <v>50</v>
       </c>
-      <c r="F18" t="s" s="11">
+      <c r="F18" t="s" s="7">
         <v>33</v>
       </c>
     </row>
     <row r="19" ht="20.05" customHeight="1">
-      <c r="A19" s="9">
+      <c r="A19" s="6">
         <v>11</v>
       </c>
-      <c r="B19" t="s" s="10">
+      <c r="B19" t="s" s="7">
         <v>36</v>
       </c>
-      <c r="C19" t="s" s="11">
+      <c r="C19" t="s" s="7">
         <v>51</v>
       </c>
-      <c r="D19" t="s" s="11">
+      <c r="D19" t="s" s="7">
         <v>52</v>
       </c>
-      <c r="E19" t="s" s="11">
+      <c r="E19" t="s" s="7">
         <v>53</v>
       </c>
-      <c r="F19" t="s" s="11">
+      <c r="F19" t="s" s="7">
         <v>54</v>
       </c>
     </row>
     <row r="20" ht="20.05" customHeight="1">
-      <c r="A20" s="9">
+      <c r="A20" s="6">
         <v>1</v>
       </c>
-      <c r="B20" t="s" s="10">
+      <c r="B20" t="s" s="7">
         <v>55</v>
       </c>
-      <c r="C20" t="s" s="11">
+      <c r="C20" t="s" s="7">
         <v>56</v>
       </c>
-      <c r="D20" t="s" s="11">
+      <c r="D20" t="s" s="7">
         <v>56</v>
       </c>
-      <c r="E20" t="s" s="11">
+      <c r="E20" t="s" s="7">
         <v>57</v>
       </c>
-      <c r="F20" t="s" s="11">
+      <c r="F20" t="s" s="7">
         <v>58</v>
       </c>
     </row>
     <row r="21" ht="20.05" customHeight="1">
-      <c r="A21" s="9">
+      <c r="A21" s="6">
         <v>1</v>
       </c>
-      <c r="B21" t="s" s="10">
+      <c r="B21" t="s" s="7">
         <v>59</v>
       </c>
-      <c r="C21" t="s" s="11">
+      <c r="C21" t="s" s="7">
         <v>60</v>
       </c>
-      <c r="D21" t="s" s="11">
+      <c r="D21" t="s" s="7">
         <v>60</v>
       </c>
-      <c r="E21" t="s" s="11">
+      <c r="E21" t="s" s="7">
         <v>61</v>
       </c>
-      <c r="F21" t="s" s="11">
+      <c r="F21" t="s" s="7">
         <v>58</v>
       </c>
     </row>
     <row r="22" ht="20.05" customHeight="1">
-      <c r="A22" s="9">
+      <c r="A22" s="6">
         <v>1</v>
       </c>
-      <c r="B22" t="s" s="10">
+      <c r="B22" t="s" s="7">
         <v>62</v>
       </c>
-      <c r="C22" t="s" s="11">
+      <c r="C22" t="s" s="7">
         <v>62</v>
       </c>
-      <c r="D22" t="s" s="11">
+      <c r="D22" t="s" s="7">
         <v>63</v>
       </c>
-      <c r="E22" t="s" s="11">
+      <c r="E22" t="s" s="7">
         <v>64</v>
       </c>
-      <c r="F22" t="s" s="11">
+      <c r="F22" t="s" s="7">
         <v>65</v>
       </c>
     </row>
     <row r="23" ht="20.05" customHeight="1">
-      <c r="A23" s="9">
+      <c r="A23" s="6">
         <v>1</v>
       </c>
-      <c r="B23" t="s" s="10">
+      <c r="B23" t="s" s="7">
         <v>66</v>
       </c>
-      <c r="C23" t="s" s="11">
+      <c r="C23" t="s" s="7">
         <v>67</v>
       </c>
-      <c r="D23" t="s" s="11">
+      <c r="D23" t="s" s="7">
         <v>68</v>
       </c>
-      <c r="E23" t="s" s="11">
+      <c r="E23" t="s" s="7">
         <v>69</v>
       </c>
-      <c r="F23" t="s" s="11">
+      <c r="F23" t="s" s="7">
         <v>66</v>
       </c>
     </row>
     <row r="24" ht="20.05" customHeight="1">
-      <c r="A24" s="9">
+      <c r="A24" s="6">
         <v>12</v>
       </c>
-      <c r="B24" t="s" s="10">
+      <c r="B24" t="s" s="7">
         <v>70</v>
       </c>
-      <c r="C24" t="s" s="11">
+      <c r="C24" t="s" s="7">
         <v>71</v>
       </c>
-      <c r="D24" t="s" s="11">
+      <c r="D24" t="s" s="7">
         <v>72</v>
       </c>
-      <c r="E24" t="s" s="11">
+      <c r="E24" t="s" s="7">
         <v>73</v>
       </c>
-      <c r="F24" t="s" s="11">
+      <c r="F24" t="s" s="7">
         <v>74</v>
       </c>
     </row>
     <row r="25" ht="20.05" customHeight="1">
-      <c r="A25" s="9">
+      <c r="A25" s="6">
         <v>1</v>
       </c>
-      <c r="B25" t="s" s="10">
+      <c r="B25" t="s" s="7">
         <v>75</v>
       </c>
-      <c r="C25" t="s" s="11">
+      <c r="C25" t="s" s="7">
         <v>75</v>
       </c>
-      <c r="D25" t="s" s="11">
+      <c r="D25" t="s" s="7">
         <v>76</v>
       </c>
-      <c r="E25" t="s" s="11">
+      <c r="E25" t="s" s="7">
         <v>77</v>
       </c>
-      <c r="F25" t="s" s="11">
+      <c r="F25" t="s" s="7">
         <v>78</v>
       </c>
     </row>
     <row r="26" ht="20.05" customHeight="1">
-      <c r="A26" s="9">
+      <c r="A26" s="6">
         <v>1</v>
       </c>
-      <c r="B26" t="s" s="10">
+      <c r="B26" t="s" s="7">
         <v>79</v>
       </c>
-      <c r="C26" t="s" s="11">
+      <c r="C26" t="s" s="7">
         <v>80</v>
       </c>
-      <c r="D26" t="s" s="11">
+      <c r="D26" t="s" s="7">
         <v>81</v>
       </c>
-      <c r="E26" t="s" s="11">
+      <c r="E26" t="s" s="7">
         <v>82</v>
       </c>
-      <c r="F26" t="s" s="11">
+      <c r="F26" t="s" s="7">
         <v>83</v>
       </c>
     </row>
     <row r="27" ht="20.05" customHeight="1">
-      <c r="A27" s="9">
+      <c r="A27" s="6">
         <v>1</v>
       </c>
-      <c r="B27" t="s" s="10">
+      <c r="B27" t="s" s="7">
         <v>84</v>
       </c>
-      <c r="C27" t="s" s="11">
+      <c r="C27" t="s" s="7">
         <v>85</v>
       </c>
-      <c r="D27" t="s" s="11">
+      <c r="D27" t="s" s="7">
         <v>86</v>
       </c>
-      <c r="E27" t="s" s="11">
+      <c r="E27" t="s" s="7">
         <v>87</v>
       </c>
-      <c r="F27" t="s" s="11">
+      <c r="F27" t="s" s="7">
         <v>88</v>
       </c>
     </row>
     <row r="28" ht="20.05" customHeight="1">
-      <c r="A28" s="9">
+      <c r="A28" s="6">
         <v>3</v>
       </c>
-      <c r="B28" t="s" s="10">
+      <c r="B28" t="s" s="7">
         <v>89</v>
       </c>
-      <c r="C28" t="s" s="11">
+      <c r="C28" t="s" s="7">
         <v>90</v>
       </c>
-      <c r="D28" t="s" s="11">
+      <c r="D28" t="s" s="7">
         <v>91</v>
       </c>
-      <c r="E28" t="s" s="11">
+      <c r="E28" t="s" s="7">
         <v>92</v>
       </c>
-      <c r="F28" t="s" s="11">
+      <c r="F28" t="s" s="7">
         <v>93</v>
       </c>
     </row>
@@ -2217,21 +2428,120 @@
       <c r="B29" t="s" s="10">
         <v>94</v>
       </c>
-      <c r="C29" t="s" s="11">
+      <c r="C29" t="s" s="10">
         <v>95</v>
       </c>
-      <c r="D29" t="s" s="11">
+      <c r="D29" t="s" s="10">
         <v>81</v>
       </c>
-      <c r="E29" t="s" s="11">
+      <c r="E29" t="s" s="10">
         <v>96</v>
       </c>
-      <c r="F29" t="s" s="11">
+      <c r="F29" t="s" s="10">
         <v>97</v>
       </c>
     </row>
+    <row r="30" ht="19.05" customHeight="1">
+      <c r="A30" t="s" s="12">
+        <v>98</v>
+      </c>
+      <c r="B30" s="13"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="14"/>
+    </row>
+    <row r="31" ht="19.05" customHeight="1">
+      <c r="A31" s="15"/>
+      <c r="B31" s="13"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="14"/>
+    </row>
+    <row r="32" ht="19.05" customHeight="1">
+      <c r="A32" s="15"/>
+      <c r="B32" s="13"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="14"/>
+    </row>
+    <row r="33" ht="19.05" customHeight="1">
+      <c r="A33" s="16"/>
+      <c r="B33" s="17"/>
+      <c r="C33" s="17"/>
+      <c r="D33" s="17"/>
+      <c r="E33" s="17"/>
+      <c r="F33" s="18"/>
+    </row>
+    <row r="34" ht="19.05" customHeight="1">
+      <c r="A34" s="19"/>
+      <c r="B34" s="19"/>
+      <c r="C34" s="19"/>
+      <c r="D34" s="19"/>
+      <c r="E34" s="19"/>
+      <c r="F34" s="20"/>
+    </row>
+    <row r="35" ht="19.05" customHeight="1">
+      <c r="A35" s="21"/>
+      <c r="B35" s="21"/>
+      <c r="C35" s="21"/>
+      <c r="D35" s="21"/>
+      <c r="E35" s="21"/>
+      <c r="F35" s="22"/>
+    </row>
+    <row r="36" ht="19.05" customHeight="1">
+      <c r="A36" s="21"/>
+      <c r="B36" s="21"/>
+      <c r="C36" s="21"/>
+      <c r="D36" s="21"/>
+      <c r="E36" s="21"/>
+      <c r="F36" s="22"/>
+    </row>
+    <row r="37" ht="19.05" customHeight="1">
+      <c r="A37" s="21"/>
+      <c r="B37" s="21"/>
+      <c r="C37" s="21"/>
+      <c r="D37" s="21"/>
+      <c r="E37" s="21"/>
+      <c r="F37" s="22"/>
+    </row>
+    <row r="38" ht="19.05" customHeight="1">
+      <c r="A38" s="21"/>
+      <c r="B38" s="21"/>
+      <c r="C38" s="21"/>
+      <c r="D38" s="21"/>
+      <c r="E38" s="21"/>
+      <c r="F38" s="22"/>
+    </row>
+    <row r="39" ht="19.05" customHeight="1">
+      <c r="A39" s="21"/>
+      <c r="B39" s="21"/>
+      <c r="C39" s="21"/>
+      <c r="D39" s="21"/>
+      <c r="E39" s="21"/>
+      <c r="F39" s="22"/>
+    </row>
+    <row r="40" ht="19.05" customHeight="1">
+      <c r="A40" s="21"/>
+      <c r="B40" s="21"/>
+      <c r="C40" s="21"/>
+      <c r="D40" s="21"/>
+      <c r="E40" s="21"/>
+      <c r="F40" s="22"/>
+    </row>
+    <row r="41" ht="19.05" customHeight="1">
+      <c r="A41" s="23"/>
+      <c r="B41" s="23"/>
+      <c r="C41" s="23"/>
+      <c r="D41" s="23"/>
+      <c r="E41" s="23"/>
+      <c r="F41" s="24"/>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
+    <mergeCell ref="A30:F41"/>
     <mergeCell ref="A1:F1"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>

</xml_diff>